<commit_message>
Additional Test cases for Create Account module
</commit_message>
<xml_diff>
--- a/target/classes/Book1.xlsx
+++ b/target/classes/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Appium_Java_Training\booking.com_App\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B593A77-EDEE-4B9E-A975-5676D6C29695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{122789EB-ACAB-49E4-80F2-483AEC31F43C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3F008BE4-AB88-4FFD-A1DF-09969BB15F96}"/>
   </bookViews>
@@ -36,7 +36,7 @@
     <t>Test$1234!</t>
   </si>
   <si>
-    <t>yes@shuramail.com</t>
+    <t>yes@finalmail.com</t>
   </si>
 </sst>
 </file>

</xml_diff>